<commit_message>
update and finalize planning and conception
</commit_message>
<xml_diff>
--- a/C61/Sprint 1/doc/C61 - Sprint1c - Outil de planification.xlsx
+++ b/C61/Sprint 1/doc/C61 - Sprint1c - Outil de planification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\---- GREEEN FLAG ----------\GreenFlag\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\---- GREEEN FLAG ----------\GreenFlag\C61\Sprint 1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D25D10-8AA2-4B52-9FD9-1ABC9FD36061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2151C904-15CF-4A72-9F7B-8A29DFE08AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -757,9 +757,6 @@
     <t>backend: abstract Strategy + AlgoStrategy</t>
   </si>
   <si>
-    <t>bibliotheque: Queue</t>
-  </si>
-  <si>
     <t>bibliotheque: middleware</t>
   </si>
   <si>
@@ -866,6 +863,9 @@
   </si>
   <si>
     <t xml:space="preserve">trigger &amp; fonction pour tableau suggestion dans la base de données </t>
+  </si>
+  <si>
+    <t>bibliotheque: DischargedList + Observer</t>
   </si>
 </sst>
 </file>
@@ -1245,11 +1245,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1265,13 +1272,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1745,7 +1745,7 @@
                   <c:v>1.8645833333294597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8854166666666743</c:v>
+                  <c:v>1.9687500000000069</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.8750000000000202</c:v>
@@ -2151,7 +2151,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8854166666666743</c:v>
+                  <c:v>1.9687500000000069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2723,7 +2723,7 @@
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2291666666628389</c:v>
+                  <c:v>7.3124999999961711</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3173,10 +3173,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5520833333333355</c:v>
+                  <c:v>1.4687500000000022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3232,10 +3232,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7291666666666843</c:v>
+                  <c:v>2.8958333333333504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3626,10 +3626,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>26</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8645833333333544</c:v>
+                  <c:v>2.7812500000000209</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3685,10 +3685,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9583333333294384</c:v>
+                  <c:v>3.1249999999961044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7519,8 +7519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.26953125" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -7542,54 +7542,54 @@
     <row r="1" spans="2:31" ht="12.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:31" ht="25.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="17"/>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" spans="2:31" ht="12.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:31" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="18"/>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="2:31" ht="6.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I6" s="15"/>
@@ -7610,12 +7610,12 @@
         <v>29</v>
       </c>
       <c r="I7" s="15"/>
-      <c r="J7" s="46" t="s">
+      <c r="J7" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
       <c r="N7" s="38">
         <v>2</v>
       </c>
@@ -7678,20 +7678,20 @@
     <row r="12" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:31" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="18"/>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
       <c r="U13" s="2">
         <f>D68</f>
         <v>48</v>
@@ -7706,12 +7706,12 @@
       <c r="C15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="5" t="s">
         <v>11</v>
       </c>
@@ -7762,12 +7762,12 @@
       <c r="C16" s="11">
         <v>1</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="30"/>
       <c r="I16" s="30" t="s">
         <v>17</v>
@@ -7806,12 +7806,12 @@
       <c r="C17" s="12">
         <v>2</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="32">
         <v>1</v>
       </c>
@@ -7875,12 +7875,12 @@
       <c r="C18" s="13">
         <v>3</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="34">
         <v>2</v>
       </c>
@@ -7941,19 +7941,19 @@
       </c>
       <c r="AE18" s="19">
         <f>SUMIFS(Duree, Sprint,AC18)</f>
-        <v>1.8854166666666743</v>
+        <v>1.9687500000000069</v>
       </c>
     </row>
     <row r="19" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C19" s="12">
         <v>4</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
       <c r="H19" s="32">
         <v>3</v>
       </c>
@@ -8021,12 +8021,12 @@
       <c r="C20" s="13">
         <v>5</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34" t="s">
         <v>17</v>
@@ -8080,12 +8080,12 @@
       <c r="C21" s="12">
         <v>6</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
       <c r="H21" s="32">
         <v>5</v>
       </c>
@@ -8126,12 +8126,12 @@
       <c r="C22" s="13">
         <v>7</v>
       </c>
-      <c r="D22" s="41" t="s">
+      <c r="D22" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
       <c r="H22" s="34">
         <v>5</v>
       </c>
@@ -8219,12 +8219,12 @@
       <c r="C24" s="13">
         <v>9</v>
       </c>
-      <c r="D24" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="D24" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
       <c r="H24" s="34"/>
       <c r="I24" s="34" t="s">
         <v>17</v>
@@ -8271,12 +8271,12 @@
       <c r="C25" s="12">
         <v>10</v>
       </c>
-      <c r="D25" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
+      <c r="D25" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
       <c r="H25" s="32">
         <v>5</v>
       </c>
@@ -8325,12 +8325,12 @@
       <c r="C26" s="13">
         <v>11</v>
       </c>
-      <c r="D26" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
+      <c r="D26" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
       <c r="H26" s="34">
         <v>10</v>
       </c>
@@ -8372,19 +8372,19 @@
       </c>
       <c r="AE26" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC26)</f>
-        <v>1.9791666666666921</v>
+        <v>2.0625000000000249</v>
       </c>
     </row>
     <row r="27" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C27" s="12">
         <v>12</v>
       </c>
-      <c r="D27" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
+      <c r="D27" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
       <c r="H27" s="32">
         <v>11</v>
       </c>
@@ -8433,12 +8433,12 @@
       <c r="C28" s="13">
         <v>13</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
       <c r="H28" s="34">
         <v>8</v>
       </c>
@@ -8487,12 +8487,12 @@
       <c r="C29" s="12">
         <v>14</v>
       </c>
-      <c r="D29" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="D29" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
       <c r="H29" s="32">
         <v>5</v>
       </c>
@@ -8529,12 +8529,12 @@
       <c r="C30" s="13">
         <v>15</v>
       </c>
-      <c r="D30" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
+      <c r="D30" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="34">
         <v>5</v>
       </c>
@@ -8577,12 +8577,12 @@
       <c r="C31" s="12">
         <v>16</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
       <c r="H31" s="32">
         <v>8</v>
       </c>
@@ -8623,19 +8623,19 @@
       </c>
       <c r="AE31" s="19">
         <f>SUMIFS(Duree, Categorie,AC31)</f>
-        <v>7.2291666666628389</v>
+        <v>7.3124999999961711</v>
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C32" s="13">
         <v>17</v>
       </c>
-      <c r="D32" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
+      <c r="D32" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
       <c r="H32" s="34">
         <v>8</v>
       </c>
@@ -8643,13 +8643,13 @@
         <v>17</v>
       </c>
       <c r="J32" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K32" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L32" s="35">
-        <v>8.3333333333333398E-2</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="M32" s="34" t="s">
         <v>14</v>
@@ -8683,12 +8683,12 @@
       <c r="C33" s="12">
         <v>18</v>
       </c>
-      <c r="D33" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
+      <c r="D33" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
       <c r="H33" s="32">
         <v>13</v>
       </c>
@@ -8736,12 +8736,12 @@
       <c r="C34" s="13">
         <v>19</v>
       </c>
-      <c r="D34" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
+      <c r="D34" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
       <c r="H34" s="34">
         <v>14</v>
       </c>
@@ -8778,12 +8778,12 @@
       <c r="C35" s="12">
         <v>20</v>
       </c>
-      <c r="D35" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
+      <c r="D35" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
       <c r="H35" s="32">
         <v>14</v>
       </c>
@@ -8826,12 +8826,12 @@
       <c r="C36" s="13">
         <v>21</v>
       </c>
-      <c r="D36" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
+      <c r="D36" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
       <c r="H36" s="34">
         <v>12</v>
       </c>
@@ -8868,23 +8868,23 @@
       </c>
       <c r="AD36" s="1">
         <f>COUNTIF(Difficulte,W17)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AE36" s="19">
         <f>SUMIFS(Duree, Difficulte,W17)</f>
-        <v>1.5520833333333355</v>
+        <v>1.4687500000000022</v>
       </c>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C37" s="12">
         <v>22</v>
       </c>
-      <c r="D37" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
+      <c r="D37" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="43"/>
       <c r="H37" s="32">
         <v>12</v>
       </c>
@@ -8921,23 +8921,23 @@
       </c>
       <c r="AD37" s="1">
         <f>COUNTIF(Difficulte,W18)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE37" s="19">
         <f>SUMIFS(Duree, Difficulte,W18)</f>
-        <v>2.7291666666666843</v>
+        <v>2.8958333333333504</v>
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C38" s="13">
         <v>23</v>
       </c>
-      <c r="D38" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
+      <c r="D38" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
       <c r="H38" s="34">
         <v>7</v>
       </c>
@@ -8985,12 +8985,12 @@
       <c r="C39" s="12">
         <v>24</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D39" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
       <c r="H39" s="32">
         <v>12</v>
       </c>
@@ -9027,12 +9027,12 @@
       <c r="C40" s="13">
         <v>25</v>
       </c>
-      <c r="D40" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
+      <c r="D40" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
       <c r="H40" s="34">
         <v>10</v>
       </c>
@@ -9075,12 +9075,12 @@
       <c r="C41" s="12">
         <v>26</v>
       </c>
-      <c r="D41" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
+      <c r="D41" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
       <c r="H41" s="32">
         <v>9</v>
       </c>
@@ -9117,23 +9117,23 @@
       </c>
       <c r="AD41" s="1">
         <f>COUNTIF(Incertitude,X17)</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AE41" s="19">
         <f>SUMIFS(Duree, Incertitude,X17)</f>
-        <v>2.8645833333333544</v>
+        <v>2.7812500000000209</v>
       </c>
     </row>
     <row r="42" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C42" s="13">
         <v>27</v>
       </c>
-      <c r="D42" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
+      <c r="D42" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
       <c r="H42" s="34">
         <v>15</v>
       </c>
@@ -9170,23 +9170,23 @@
       </c>
       <c r="AD42" s="1">
         <f>COUNTIF(Incertitude,X18)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE42" s="19">
         <f>SUMIFS(Duree, Incertitude,X18)</f>
-        <v>2.9583333333294384</v>
+        <v>3.1249999999961044</v>
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C43" s="12">
         <v>28</v>
       </c>
-      <c r="D43" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
+      <c r="D43" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
       <c r="H43" s="32">
         <v>10</v>
       </c>
@@ -9234,12 +9234,12 @@
       <c r="C44" s="13">
         <v>29</v>
       </c>
-      <c r="D44" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
+      <c r="D44" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
       <c r="H44" s="34">
         <v>15</v>
       </c>
@@ -9276,12 +9276,12 @@
       <c r="C45" s="12">
         <v>30</v>
       </c>
-      <c r="D45" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
+      <c r="D45" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
       <c r="H45" s="32">
         <v>24</v>
       </c>
@@ -9318,12 +9318,12 @@
       <c r="C46" s="13">
         <v>31</v>
       </c>
-      <c r="D46" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
+      <c r="D46" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
       <c r="H46" s="34">
         <v>10</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>32</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E47" s="29"/>
       <c r="F47" s="29"/>
@@ -9402,12 +9402,12 @@
       <c r="C48" s="13">
         <v>33</v>
       </c>
-      <c r="D48" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
+      <c r="D48" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
       <c r="H48" s="34">
         <v>21</v>
       </c>
@@ -9444,12 +9444,12 @@
       <c r="C49" s="12">
         <v>34</v>
       </c>
-      <c r="D49" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
+      <c r="D49" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
       <c r="H49" s="32">
         <v>12</v>
       </c>
@@ -9489,12 +9489,12 @@
       <c r="C50" s="13">
         <v>35</v>
       </c>
-      <c r="D50" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
+      <c r="D50" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
       <c r="H50" s="34">
         <v>21</v>
       </c>
@@ -9534,12 +9534,12 @@
       <c r="C51" s="12">
         <v>36</v>
       </c>
-      <c r="D51" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
+      <c r="D51" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
       <c r="H51" s="32">
         <v>23</v>
       </c>
@@ -9579,12 +9579,12 @@
       <c r="C52" s="13">
         <v>37</v>
       </c>
-      <c r="D52" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="41"/>
+      <c r="D52" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
       <c r="H52" s="34">
         <v>19</v>
       </c>
@@ -9624,12 +9624,12 @@
       <c r="C53" s="12">
         <v>38</v>
       </c>
-      <c r="D53" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
+      <c r="D53" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
       <c r="H53" s="32">
         <v>13</v>
       </c>
@@ -9669,12 +9669,12 @@
       <c r="C54" s="13">
         <v>39</v>
       </c>
-      <c r="D54" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
+      <c r="D54" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
       <c r="H54" s="34">
         <v>10</v>
       </c>
@@ -9714,12 +9714,12 @@
       <c r="C55" s="12">
         <v>40</v>
       </c>
-      <c r="D55" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
+      <c r="D55" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
       <c r="H55" s="32">
         <v>26</v>
       </c>
@@ -9759,12 +9759,12 @@
       <c r="C56" s="13">
         <v>41</v>
       </c>
-      <c r="D56" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
+      <c r="D56" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
       <c r="H56" s="34">
         <v>16</v>
       </c>
@@ -9804,12 +9804,12 @@
       <c r="C57" s="12">
         <v>42</v>
       </c>
-      <c r="D57" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
+      <c r="D57" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="43"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="43"/>
       <c r="H57" s="32">
         <v>35</v>
       </c>
@@ -9849,12 +9849,12 @@
       <c r="C58" s="13">
         <v>43</v>
       </c>
-      <c r="D58" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
-      <c r="G58" s="41"/>
+      <c r="D58" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
       <c r="H58" s="34">
         <v>13</v>
       </c>
@@ -9894,12 +9894,12 @@
       <c r="C59" s="12">
         <v>44</v>
       </c>
-      <c r="D59" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
+      <c r="D59" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
       <c r="H59" s="32"/>
       <c r="I59" s="32" t="s">
         <v>18</v>
@@ -9937,12 +9937,12 @@
       <c r="C60" s="13">
         <v>45</v>
       </c>
-      <c r="D60" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
+      <c r="D60" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
       <c r="H60" s="34">
         <v>11</v>
       </c>
@@ -9982,12 +9982,12 @@
       <c r="C61" s="12">
         <v>46</v>
       </c>
-      <c r="D61" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
+      <c r="D61" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
       <c r="H61" s="32"/>
       <c r="I61" s="32" t="s">
         <v>17</v>
@@ -10025,12 +10025,12 @@
       <c r="C62" s="13">
         <v>47</v>
       </c>
-      <c r="D62" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="E62" s="41"/>
-      <c r="F62" s="41"/>
-      <c r="G62" s="41"/>
+      <c r="D62" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
       <c r="H62" s="34"/>
       <c r="I62" s="34" t="s">
         <v>17</v>
@@ -10068,12 +10068,12 @@
       <c r="C63" s="12">
         <v>48</v>
       </c>
-      <c r="D63" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
+      <c r="D63" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
       <c r="H63" s="32"/>
       <c r="I63" s="32" t="s">
         <v>17</v>
@@ -10111,10 +10111,10 @@
       <c r="C64" s="13">
         <v>49</v>
       </c>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
-      <c r="F64" s="41"/>
-      <c r="G64" s="41"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
@@ -10140,10 +10140,10 @@
       <c r="C65" s="14">
         <v>50</v>
       </c>
-      <c r="D65" s="42"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
       <c r="H65" s="36"/>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
@@ -10204,7 +10204,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="9">
         <f>SUM(L16:L65)</f>
-        <v>8.0520833333295023</v>
+        <v>8.1354166666628345</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -10483,44 +10483,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tjqSiT+XspradLJBNpu0viI4TokIDIF0O7QeXm3BTZLmeAfSOw5TlniSFfStQ9LXJLtK7gLyf3B6jINr+qJ+Cg==" saltValue="/wSmyHkNAfBsPbW8NILu1w==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="54">
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G50"/>
     <mergeCell ref="D63:G63"/>
     <mergeCell ref="D64:G64"/>
     <mergeCell ref="D65:G65"/>
@@ -10537,6 +10499,44 @@
     <mergeCell ref="D62:G62"/>
     <mergeCell ref="D51:G51"/>
     <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D50:G50"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:N2">
     <cfRule type="expression" dxfId="9" priority="3">
@@ -10661,14 +10661,14 @@
   <sheetData>
     <row r="1" spans="2:13" ht="13" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="2:13" ht="10.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10724,7 +10724,7 @@
       </c>
       <c r="D6" s="10">
         <f>SUMIFS(Duree, Sprint,D4)</f>
-        <v>1.8854166666666743</v>
+        <v>1.9687500000000069</v>
       </c>
       <c r="E6" s="10">
         <f>SUMIFS(Duree, Sprint,E4)</f>
@@ -10736,7 +10736,7 @@
       </c>
       <c r="G6" s="26">
         <f>SUM(C6:F6)</f>
-        <v>8.0520833333295023</v>
+        <v>8.1354166666628362</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>